<commit_message>
avance en analisis sql
</commit_message>
<xml_diff>
--- a/UPGRADE 3100-5000.xlsx
+++ b/UPGRADE 3100-5000.xlsx
@@ -1196,8 +1196,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1236,53 +1236,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1297,46 +1253,27 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1350,15 +1287,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1373,17 +1334,56 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -1479,7 +1479,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1491,19 +1557,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1515,25 +1581,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1545,7 +1611,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1557,91 +1635,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1873,11 +1873,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1887,6 +1902,30 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1917,21 +1956,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1946,40 +1970,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1994,128 +1994,128 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2738,11 +2738,11 @@
   <dimension ref="A1:DP685"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="I1" workbookViewId="0">
-      <pane xSplit="5745" ySplit="1170" topLeftCell="BV16" activePane="bottomRight"/>
+      <pane xSplit="5745" ySplit="1170" topLeftCell="CH70" activePane="bottomRight"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="CR65" sqref="CR65"/>
+      <selection pane="bottomRight" activeCell="DC80" sqref="DC80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4285714285714" defaultRowHeight="11.25"/>
@@ -5283,15 +5283,15 @@
       </c>
       <c r="K17" s="24">
         <f t="shared" ref="K17:K21" si="0">MAX(AH18:DP18)</f>
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L17" s="49">
         <f t="shared" ref="L17:L21" si="1">J17-K17</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M17" s="24">
         <f>K17-K19</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N17" s="24">
         <v>1</v>
@@ -5826,16 +5826,36 @@
       <c r="CR18" s="60">
         <v>85</v>
       </c>
-      <c r="CS18" s="60"/>
-      <c r="CT18" s="60"/>
-      <c r="CU18" s="60"/>
-      <c r="CV18" s="60"/>
-      <c r="CW18" s="60"/>
-      <c r="CX18" s="60"/>
-      <c r="CY18" s="60"/>
-      <c r="CZ18" s="60"/>
-      <c r="DA18" s="60"/>
-      <c r="DB18" s="60"/>
+      <c r="CS18" s="60">
+        <v>85</v>
+      </c>
+      <c r="CT18" s="60">
+        <v>85</v>
+      </c>
+      <c r="CU18" s="60">
+        <v>85</v>
+      </c>
+      <c r="CV18" s="60">
+        <v>85</v>
+      </c>
+      <c r="CW18" s="60">
+        <v>85</v>
+      </c>
+      <c r="CX18" s="60">
+        <v>85</v>
+      </c>
+      <c r="CY18" s="60">
+        <v>86</v>
+      </c>
+      <c r="CZ18" s="60">
+        <v>86</v>
+      </c>
+      <c r="DA18" s="60">
+        <v>86</v>
+      </c>
+      <c r="DB18" s="60">
+        <v>88</v>
+      </c>
       <c r="DC18" s="60"/>
       <c r="DD18" s="60"/>
       <c r="DE18" s="60"/>
@@ -5885,15 +5905,15 @@
       </c>
       <c r="K19" s="29">
         <f t="shared" si="0"/>
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L19" s="51">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M19" s="29">
         <f>K19-K21</f>
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N19" s="29">
         <v>1</v>
@@ -6426,16 +6446,36 @@
       <c r="CR20" s="43">
         <v>83</v>
       </c>
-      <c r="CS20" s="43"/>
-      <c r="CT20" s="43"/>
-      <c r="CU20" s="43"/>
-      <c r="CV20" s="43"/>
-      <c r="CW20" s="43"/>
-      <c r="CX20" s="43"/>
-      <c r="CY20" s="43"/>
-      <c r="CZ20" s="43"/>
-      <c r="DA20" s="43"/>
-      <c r="DB20" s="43"/>
+      <c r="CS20" s="43">
+        <v>83</v>
+      </c>
+      <c r="CT20" s="43">
+        <v>83</v>
+      </c>
+      <c r="CU20" s="43">
+        <v>83</v>
+      </c>
+      <c r="CV20" s="43">
+        <v>84</v>
+      </c>
+      <c r="CW20" s="43">
+        <v>84</v>
+      </c>
+      <c r="CX20" s="43">
+        <v>84</v>
+      </c>
+      <c r="CY20" s="43">
+        <v>84</v>
+      </c>
+      <c r="CZ20" s="43">
+        <v>84</v>
+      </c>
+      <c r="DA20" s="43">
+        <v>84</v>
+      </c>
+      <c r="DB20" s="43">
+        <v>84</v>
+      </c>
       <c r="DC20" s="43"/>
       <c r="DD20" s="43"/>
       <c r="DE20" s="43"/>
@@ -6743,15 +6783,15 @@
       </c>
       <c r="K23" s="24">
         <f t="shared" ref="K23:K27" si="7">MAX(AH24:DP24)</f>
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="L23" s="49">
         <f t="shared" ref="L23:L27" si="8">J23-K23</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M23" s="24">
         <f>K23-K25</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N23" s="24">
         <v>1</v>
@@ -7208,16 +7248,36 @@
       <c r="CR24" s="43">
         <v>64</v>
       </c>
-      <c r="CS24" s="43"/>
-      <c r="CT24" s="43"/>
-      <c r="CU24" s="43"/>
-      <c r="CV24" s="43"/>
-      <c r="CW24" s="43"/>
-      <c r="CX24" s="43"/>
-      <c r="CY24" s="43"/>
-      <c r="CZ24" s="43"/>
-      <c r="DA24" s="43"/>
-      <c r="DB24" s="43"/>
+      <c r="CS24" s="43">
+        <v>65</v>
+      </c>
+      <c r="CT24" s="43">
+        <v>65</v>
+      </c>
+      <c r="CU24" s="43">
+        <v>65</v>
+      </c>
+      <c r="CV24" s="43">
+        <v>67</v>
+      </c>
+      <c r="CW24" s="43">
+        <v>67</v>
+      </c>
+      <c r="CX24" s="43">
+        <v>67</v>
+      </c>
+      <c r="CY24" s="43">
+        <v>67</v>
+      </c>
+      <c r="CZ24" s="43">
+        <v>68</v>
+      </c>
+      <c r="DA24" s="43">
+        <v>70</v>
+      </c>
+      <c r="DB24" s="43">
+        <v>68</v>
+      </c>
       <c r="DC24" s="43"/>
       <c r="DD24" s="43"/>
       <c r="DE24" s="43"/>
@@ -7263,15 +7323,15 @@
       </c>
       <c r="K25" s="29">
         <f t="shared" si="7"/>
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L25" s="51">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M25" s="29">
         <f>K25-K27</f>
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="N25" s="29">
         <v>1</v>
@@ -7726,16 +7786,36 @@
       <c r="CR26" s="43">
         <v>61</v>
       </c>
-      <c r="CS26" s="43"/>
-      <c r="CT26" s="43"/>
-      <c r="CU26" s="43"/>
-      <c r="CV26" s="43"/>
-      <c r="CW26" s="43"/>
-      <c r="CX26" s="43"/>
-      <c r="CY26" s="43"/>
-      <c r="CZ26" s="43"/>
-      <c r="DA26" s="43"/>
-      <c r="DB26" s="43"/>
+      <c r="CS26" s="43">
+        <v>61</v>
+      </c>
+      <c r="CT26" s="43">
+        <v>61</v>
+      </c>
+      <c r="CU26" s="43">
+        <v>61</v>
+      </c>
+      <c r="CV26" s="43">
+        <v>61</v>
+      </c>
+      <c r="CW26" s="43">
+        <v>61</v>
+      </c>
+      <c r="CX26" s="43">
+        <v>61</v>
+      </c>
+      <c r="CY26" s="43">
+        <v>61</v>
+      </c>
+      <c r="CZ26" s="43">
+        <v>62</v>
+      </c>
+      <c r="DA26" s="43">
+        <v>63</v>
+      </c>
+      <c r="DB26" s="43">
+        <v>63</v>
+      </c>
       <c r="DC26" s="43"/>
       <c r="DD26" s="43"/>
       <c r="DE26" s="43"/>
@@ -8051,7 +8131,7 @@
       </c>
       <c r="M29" s="24">
         <f>K29-K31</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N29" s="24">
         <v>2</v>
@@ -8628,16 +8708,36 @@
       <c r="CR30" s="43">
         <v>137</v>
       </c>
-      <c r="CS30" s="43"/>
-      <c r="CT30" s="43"/>
-      <c r="CU30" s="43"/>
-      <c r="CV30" s="43"/>
-      <c r="CW30" s="43"/>
-      <c r="CX30" s="43"/>
-      <c r="CY30" s="43"/>
-      <c r="CZ30" s="43"/>
-      <c r="DA30" s="43"/>
-      <c r="DB30" s="43"/>
+      <c r="CS30" s="43">
+        <v>138</v>
+      </c>
+      <c r="CT30" s="43">
+        <v>139</v>
+      </c>
+      <c r="CU30" s="43">
+        <v>139</v>
+      </c>
+      <c r="CV30" s="43">
+        <v>139</v>
+      </c>
+      <c r="CW30" s="43">
+        <v>139</v>
+      </c>
+      <c r="CX30" s="43">
+        <v>139</v>
+      </c>
+      <c r="CY30" s="43">
+        <v>140</v>
+      </c>
+      <c r="CZ30" s="43">
+        <v>140</v>
+      </c>
+      <c r="DA30" s="43">
+        <v>140</v>
+      </c>
+      <c r="DB30" s="43">
+        <v>140</v>
+      </c>
       <c r="DC30" s="43"/>
       <c r="DD30" s="43"/>
       <c r="DE30" s="43"/>
@@ -8683,15 +8783,15 @@
       </c>
       <c r="K31" s="29">
         <f t="shared" si="11"/>
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L31" s="51">
         <f t="shared" si="12"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M31" s="29">
         <f>K31-K33</f>
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="N31" s="29">
         <v>2</v>
@@ -9266,16 +9366,36 @@
       <c r="CR32" s="43">
         <v>135</v>
       </c>
-      <c r="CS32" s="43"/>
-      <c r="CT32" s="43"/>
-      <c r="CU32" s="43"/>
-      <c r="CV32" s="43"/>
-      <c r="CW32" s="43"/>
-      <c r="CX32" s="43"/>
-      <c r="CY32" s="43"/>
-      <c r="CZ32" s="43"/>
-      <c r="DA32" s="43"/>
-      <c r="DB32" s="43"/>
+      <c r="CS32" s="43">
+        <v>135</v>
+      </c>
+      <c r="CT32" s="43">
+        <v>136</v>
+      </c>
+      <c r="CU32" s="43">
+        <v>136</v>
+      </c>
+      <c r="CV32" s="43">
+        <v>136</v>
+      </c>
+      <c r="CW32" s="43">
+        <v>136</v>
+      </c>
+      <c r="CX32" s="43">
+        <v>136</v>
+      </c>
+      <c r="CY32" s="43">
+        <v>136</v>
+      </c>
+      <c r="CZ32" s="43">
+        <v>136</v>
+      </c>
+      <c r="DA32" s="43">
+        <v>136</v>
+      </c>
+      <c r="DB32" s="43">
+        <v>136</v>
+      </c>
       <c r="DC32" s="43"/>
       <c r="DD32" s="43"/>
       <c r="DE32" s="43"/>
@@ -9579,15 +9699,15 @@
       </c>
       <c r="K35" s="24">
         <f t="shared" ref="K35:K39" si="18">MAX(AH36:DP36)</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L35" s="49">
         <f t="shared" ref="L35:L39" si="19">J35-K35</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M35" s="24">
         <f>K35-K37</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N35" s="24">
         <v>1</v>
@@ -10095,16 +10215,36 @@
       <c r="CR36" s="43">
         <v>45</v>
       </c>
-      <c r="CS36" s="43"/>
-      <c r="CT36" s="43"/>
-      <c r="CU36" s="43"/>
-      <c r="CV36" s="43"/>
-      <c r="CW36" s="43"/>
-      <c r="CX36" s="43"/>
-      <c r="CY36" s="43"/>
-      <c r="CZ36" s="43"/>
-      <c r="DA36" s="43"/>
-      <c r="DB36" s="43"/>
+      <c r="CS36" s="43">
+        <v>45</v>
+      </c>
+      <c r="CT36" s="43">
+        <v>45</v>
+      </c>
+      <c r="CU36" s="43">
+        <v>45</v>
+      </c>
+      <c r="CV36" s="43">
+        <v>45</v>
+      </c>
+      <c r="CW36" s="43">
+        <v>45</v>
+      </c>
+      <c r="CX36" s="43">
+        <v>45</v>
+      </c>
+      <c r="CY36" s="43">
+        <v>45</v>
+      </c>
+      <c r="CZ36" s="43">
+        <v>46</v>
+      </c>
+      <c r="DA36" s="43">
+        <v>46</v>
+      </c>
+      <c r="DB36" s="43">
+        <v>46</v>
+      </c>
       <c r="DC36" s="43"/>
       <c r="DD36" s="43"/>
       <c r="DE36" s="43"/>
@@ -10662,16 +10802,36 @@
       <c r="CR38" s="43">
         <v>43</v>
       </c>
-      <c r="CS38" s="43"/>
-      <c r="CT38" s="43"/>
-      <c r="CU38" s="43"/>
-      <c r="CV38" s="43"/>
-      <c r="CW38" s="43"/>
-      <c r="CX38" s="43"/>
-      <c r="CY38" s="43"/>
-      <c r="CZ38" s="43"/>
-      <c r="DA38" s="43"/>
-      <c r="DB38" s="43"/>
+      <c r="CS38" s="43">
+        <v>43</v>
+      </c>
+      <c r="CT38" s="43">
+        <v>43</v>
+      </c>
+      <c r="CU38" s="43">
+        <v>43</v>
+      </c>
+      <c r="CV38" s="43">
+        <v>43</v>
+      </c>
+      <c r="CW38" s="43">
+        <v>43</v>
+      </c>
+      <c r="CX38" s="43">
+        <v>43</v>
+      </c>
+      <c r="CY38" s="43">
+        <v>43</v>
+      </c>
+      <c r="CZ38" s="43">
+        <v>44</v>
+      </c>
+      <c r="DA38" s="43">
+        <v>44</v>
+      </c>
+      <c r="DB38" s="43">
+        <v>44</v>
+      </c>
       <c r="DC38" s="43"/>
       <c r="DD38" s="43"/>
       <c r="DE38" s="43"/>
@@ -10977,15 +11137,15 @@
       </c>
       <c r="K41" s="24">
         <f t="shared" ref="K41:K45" si="23">MAX(AH42:DP42)</f>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L41" s="49">
         <f t="shared" ref="L41:L45" si="24">J41-K41</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M41" s="24">
         <f>K41-K43</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N41" s="24">
         <v>1</v>
@@ -11489,16 +11649,36 @@
       <c r="CR42" s="43">
         <v>51</v>
       </c>
-      <c r="CS42" s="43"/>
-      <c r="CT42" s="43"/>
-      <c r="CU42" s="43"/>
-      <c r="CV42" s="43"/>
-      <c r="CW42" s="43"/>
-      <c r="CX42" s="43"/>
-      <c r="CY42" s="43"/>
-      <c r="CZ42" s="43"/>
-      <c r="DA42" s="43"/>
-      <c r="DB42" s="43"/>
+      <c r="CS42" s="43">
+        <v>51</v>
+      </c>
+      <c r="CT42" s="43">
+        <v>51</v>
+      </c>
+      <c r="CU42" s="43">
+        <v>51</v>
+      </c>
+      <c r="CV42" s="43">
+        <v>51</v>
+      </c>
+      <c r="CW42" s="43">
+        <v>51</v>
+      </c>
+      <c r="CX42" s="43">
+        <v>51</v>
+      </c>
+      <c r="CY42" s="43">
+        <v>51</v>
+      </c>
+      <c r="CZ42" s="43">
+        <v>52</v>
+      </c>
+      <c r="DA42" s="43">
+        <v>52</v>
+      </c>
+      <c r="DB42" s="43">
+        <v>52</v>
+      </c>
       <c r="DC42" s="43"/>
       <c r="DD42" s="43"/>
       <c r="DE42" s="43"/>
@@ -12052,16 +12232,36 @@
       <c r="CR44" s="43">
         <v>49</v>
       </c>
-      <c r="CS44" s="43"/>
-      <c r="CT44" s="43"/>
-      <c r="CU44" s="43"/>
-      <c r="CV44" s="43"/>
-      <c r="CW44" s="43"/>
-      <c r="CX44" s="43"/>
-      <c r="CY44" s="43"/>
-      <c r="CZ44" s="43"/>
-      <c r="DA44" s="43"/>
-      <c r="DB44" s="43"/>
+      <c r="CS44" s="43">
+        <v>49</v>
+      </c>
+      <c r="CT44" s="43">
+        <v>49</v>
+      </c>
+      <c r="CU44" s="43">
+        <v>49</v>
+      </c>
+      <c r="CV44" s="43">
+        <v>49</v>
+      </c>
+      <c r="CW44" s="43">
+        <v>49</v>
+      </c>
+      <c r="CX44" s="43">
+        <v>49</v>
+      </c>
+      <c r="CY44" s="43">
+        <v>49</v>
+      </c>
+      <c r="CZ44" s="43">
+        <v>49</v>
+      </c>
+      <c r="DA44" s="43">
+        <v>49</v>
+      </c>
+      <c r="DB44" s="43">
+        <v>49</v>
+      </c>
       <c r="DC44" s="43"/>
       <c r="DD44" s="43"/>
       <c r="DE44" s="43"/>
@@ -12367,15 +12567,15 @@
       </c>
       <c r="K47" s="24">
         <f t="shared" ref="K47:K51" si="28">MAX(AH48:DP48)</f>
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="L47" s="49">
         <f t="shared" ref="L47:L51" si="29">J47-K47</f>
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="M47" s="24">
         <f>K47-K49</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="N47" s="24">
         <v>2</v>
@@ -12945,16 +13145,36 @@
       <c r="CR48" s="43">
         <v>137</v>
       </c>
-      <c r="CS48" s="43"/>
-      <c r="CT48" s="43"/>
-      <c r="CU48" s="43"/>
-      <c r="CV48" s="43"/>
-      <c r="CW48" s="43"/>
-      <c r="CX48" s="43"/>
-      <c r="CY48" s="43"/>
-      <c r="CZ48" s="43"/>
-      <c r="DA48" s="43"/>
-      <c r="DB48" s="43"/>
+      <c r="CS48" s="43">
+        <v>137</v>
+      </c>
+      <c r="CT48" s="43">
+        <v>138</v>
+      </c>
+      <c r="CU48" s="43">
+        <v>139</v>
+      </c>
+      <c r="CV48" s="43">
+        <v>139</v>
+      </c>
+      <c r="CW48" s="43">
+        <v>139</v>
+      </c>
+      <c r="CX48" s="43">
+        <v>139</v>
+      </c>
+      <c r="CY48" s="43">
+        <v>139</v>
+      </c>
+      <c r="CZ48" s="43">
+        <v>143</v>
+      </c>
+      <c r="DA48" s="43">
+        <v>145</v>
+      </c>
+      <c r="DB48" s="43">
+        <v>143</v>
+      </c>
       <c r="DC48" s="43"/>
       <c r="DD48" s="43"/>
       <c r="DE48" s="43"/>
@@ -12998,15 +13218,15 @@
       </c>
       <c r="K49" s="29">
         <f t="shared" si="28"/>
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="L49" s="51">
         <f t="shared" si="29"/>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="M49" s="29">
         <f>K49-K51</f>
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="N49" s="29">
         <v>2</v>
@@ -13574,16 +13794,36 @@
       <c r="CR50" s="43">
         <v>131</v>
       </c>
-      <c r="CS50" s="43"/>
-      <c r="CT50" s="43"/>
-      <c r="CU50" s="43"/>
-      <c r="CV50" s="43"/>
-      <c r="CW50" s="43"/>
-      <c r="CX50" s="43"/>
-      <c r="CY50" s="43"/>
-      <c r="CZ50" s="43"/>
-      <c r="DA50" s="43"/>
-      <c r="DB50" s="43"/>
+      <c r="CS50" s="43">
+        <v>131</v>
+      </c>
+      <c r="CT50" s="43">
+        <v>131</v>
+      </c>
+      <c r="CU50" s="43">
+        <v>131</v>
+      </c>
+      <c r="CV50" s="43">
+        <v>131</v>
+      </c>
+      <c r="CW50" s="43">
+        <v>131</v>
+      </c>
+      <c r="CX50" s="43">
+        <v>131</v>
+      </c>
+      <c r="CY50" s="43">
+        <v>131</v>
+      </c>
+      <c r="CZ50" s="43">
+        <v>133</v>
+      </c>
+      <c r="DA50" s="43">
+        <v>133</v>
+      </c>
+      <c r="DB50" s="43">
+        <v>135</v>
+      </c>
       <c r="DC50" s="43"/>
       <c r="DD50" s="43"/>
       <c r="DE50" s="43"/>
@@ -14246,16 +14486,36 @@
       <c r="CR54" s="43">
         <v>24</v>
       </c>
-      <c r="CS54" s="43"/>
-      <c r="CT54" s="43"/>
-      <c r="CU54" s="43"/>
-      <c r="CV54" s="43"/>
-      <c r="CW54" s="43"/>
-      <c r="CX54" s="43"/>
-      <c r="CY54" s="43"/>
-      <c r="CZ54" s="43"/>
-      <c r="DA54" s="43"/>
-      <c r="DB54" s="43"/>
+      <c r="CS54" s="43">
+        <v>24</v>
+      </c>
+      <c r="CT54" s="43">
+        <v>24</v>
+      </c>
+      <c r="CU54" s="43">
+        <v>24</v>
+      </c>
+      <c r="CV54" s="43">
+        <v>24</v>
+      </c>
+      <c r="CW54" s="43">
+        <v>24</v>
+      </c>
+      <c r="CX54" s="43">
+        <v>24</v>
+      </c>
+      <c r="CY54" s="43">
+        <v>24</v>
+      </c>
+      <c r="CZ54" s="43">
+        <v>24</v>
+      </c>
+      <c r="DA54" s="43">
+        <v>24</v>
+      </c>
+      <c r="DB54" s="43">
+        <v>24</v>
+      </c>
       <c r="DC54" s="43"/>
       <c r="DD54" s="43"/>
       <c r="DE54" s="43"/>
@@ -14654,16 +14914,36 @@
       <c r="CR56" s="43">
         <v>24</v>
       </c>
-      <c r="CS56" s="43"/>
-      <c r="CT56" s="43"/>
-      <c r="CU56" s="43"/>
-      <c r="CV56" s="43"/>
-      <c r="CW56" s="43"/>
-      <c r="CX56" s="43"/>
-      <c r="CY56" s="43"/>
-      <c r="CZ56" s="43"/>
-      <c r="DA56" s="43"/>
-      <c r="DB56" s="43"/>
+      <c r="CS56" s="43">
+        <v>24</v>
+      </c>
+      <c r="CT56" s="43">
+        <v>24</v>
+      </c>
+      <c r="CU56" s="43">
+        <v>24</v>
+      </c>
+      <c r="CV56" s="43">
+        <v>24</v>
+      </c>
+      <c r="CW56" s="43">
+        <v>24</v>
+      </c>
+      <c r="CX56" s="43">
+        <v>24</v>
+      </c>
+      <c r="CY56" s="43">
+        <v>24</v>
+      </c>
+      <c r="CZ56" s="43">
+        <v>24</v>
+      </c>
+      <c r="DA56" s="43">
+        <v>24</v>
+      </c>
+      <c r="DB56" s="43">
+        <v>24</v>
+      </c>
       <c r="DC56" s="43"/>
       <c r="DD56" s="43"/>
       <c r="DE56" s="43"/>
@@ -15252,16 +15532,36 @@
       <c r="CR60" s="43">
         <v>8</v>
       </c>
-      <c r="CS60" s="43"/>
-      <c r="CT60" s="43"/>
-      <c r="CU60" s="43"/>
-      <c r="CV60" s="43"/>
-      <c r="CW60" s="43"/>
-      <c r="CX60" s="43"/>
-      <c r="CY60" s="43"/>
-      <c r="CZ60" s="43"/>
-      <c r="DA60" s="43"/>
-      <c r="DB60" s="43"/>
+      <c r="CS60" s="43">
+        <v>8</v>
+      </c>
+      <c r="CT60" s="43">
+        <v>8</v>
+      </c>
+      <c r="CU60" s="43">
+        <v>8</v>
+      </c>
+      <c r="CV60" s="43">
+        <v>8</v>
+      </c>
+      <c r="CW60" s="43">
+        <v>8</v>
+      </c>
+      <c r="CX60" s="43">
+        <v>8</v>
+      </c>
+      <c r="CY60" s="43">
+        <v>8</v>
+      </c>
+      <c r="CZ60" s="43">
+        <v>8</v>
+      </c>
+      <c r="DA60" s="43">
+        <v>8</v>
+      </c>
+      <c r="DB60" s="43">
+        <v>8</v>
+      </c>
       <c r="DC60" s="43"/>
       <c r="DD60" s="43"/>
       <c r="DE60" s="43"/>
@@ -15638,16 +15938,36 @@
       <c r="CR62" s="43">
         <v>8</v>
       </c>
-      <c r="CS62" s="43"/>
-      <c r="CT62" s="43"/>
-      <c r="CU62" s="43"/>
-      <c r="CV62" s="43"/>
-      <c r="CW62" s="43"/>
-      <c r="CX62" s="43"/>
-      <c r="CY62" s="43"/>
-      <c r="CZ62" s="43"/>
-      <c r="DA62" s="43"/>
-      <c r="DB62" s="43"/>
+      <c r="CS62" s="43">
+        <v>8</v>
+      </c>
+      <c r="CT62" s="43">
+        <v>8</v>
+      </c>
+      <c r="CU62" s="43">
+        <v>8</v>
+      </c>
+      <c r="CV62" s="43">
+        <v>8</v>
+      </c>
+      <c r="CW62" s="43">
+        <v>8</v>
+      </c>
+      <c r="CX62" s="43">
+        <v>8</v>
+      </c>
+      <c r="CY62" s="43">
+        <v>8</v>
+      </c>
+      <c r="CZ62" s="43">
+        <v>8</v>
+      </c>
+      <c r="DA62" s="43">
+        <v>8</v>
+      </c>
+      <c r="DB62" s="43">
+        <v>8</v>
+      </c>
       <c r="DC62" s="43"/>
       <c r="DD62" s="43"/>
       <c r="DE62" s="43"/>
@@ -15961,7 +16281,7 @@
       </c>
       <c r="M65" s="24">
         <f>K65-K67</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N65" s="24">
         <v>0</v>
@@ -16214,16 +16534,36 @@
       <c r="CR66" s="43">
         <v>1</v>
       </c>
-      <c r="CS66" s="43"/>
-      <c r="CT66" s="43"/>
-      <c r="CU66" s="43"/>
-      <c r="CV66" s="43"/>
-      <c r="CW66" s="43"/>
-      <c r="CX66" s="43"/>
-      <c r="CY66" s="43"/>
-      <c r="CZ66" s="43"/>
-      <c r="DA66" s="43"/>
-      <c r="DB66" s="43"/>
+      <c r="CS66" s="43">
+        <v>1</v>
+      </c>
+      <c r="CT66" s="43">
+        <v>1</v>
+      </c>
+      <c r="CU66" s="43">
+        <v>1</v>
+      </c>
+      <c r="CV66" s="43">
+        <v>1</v>
+      </c>
+      <c r="CW66" s="43">
+        <v>1</v>
+      </c>
+      <c r="CX66" s="43">
+        <v>1</v>
+      </c>
+      <c r="CY66" s="43">
+        <v>1</v>
+      </c>
+      <c r="CZ66" s="43">
+        <v>1</v>
+      </c>
+      <c r="DA66" s="43">
+        <v>2</v>
+      </c>
+      <c r="DB66" s="43">
+        <v>2</v>
+      </c>
       <c r="DC66" s="43"/>
       <c r="DD66" s="43"/>
       <c r="DE66" s="43"/>
@@ -16267,15 +16607,15 @@
       </c>
       <c r="K67" s="29">
         <f t="shared" si="41"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L67" s="51">
         <f t="shared" si="42"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M67" s="29">
         <f>K67-K69</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N67" s="29">
         <v>0</v>
@@ -16526,16 +16866,36 @@
       <c r="CR68" s="43">
         <v>1</v>
       </c>
-      <c r="CS68" s="43"/>
-      <c r="CT68" s="43"/>
-      <c r="CU68" s="43"/>
-      <c r="CV68" s="43"/>
-      <c r="CW68" s="43"/>
-      <c r="CX68" s="43"/>
-      <c r="CY68" s="43"/>
-      <c r="CZ68" s="43"/>
-      <c r="DA68" s="43"/>
-      <c r="DB68" s="43"/>
+      <c r="CS68" s="43">
+        <v>1</v>
+      </c>
+      <c r="CT68" s="43">
+        <v>1</v>
+      </c>
+      <c r="CU68" s="43">
+        <v>1</v>
+      </c>
+      <c r="CV68" s="43">
+        <v>1</v>
+      </c>
+      <c r="CW68" s="43">
+        <v>1</v>
+      </c>
+      <c r="CX68" s="43">
+        <v>1</v>
+      </c>
+      <c r="CY68" s="43">
+        <v>1</v>
+      </c>
+      <c r="CZ68" s="43">
+        <v>1</v>
+      </c>
+      <c r="DA68" s="43">
+        <v>2</v>
+      </c>
+      <c r="DB68" s="43">
+        <v>2</v>
+      </c>
       <c r="DC68" s="43"/>
       <c r="DD68" s="43"/>
       <c r="DE68" s="43"/>
@@ -16841,15 +17201,15 @@
       </c>
       <c r="K71" s="24">
         <f t="shared" ref="K71:K75" si="43">MAX(AH72:DP72)</f>
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L71" s="49">
         <f t="shared" ref="L71:L75" si="44">J71-K71</f>
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M71" s="24">
         <f>K71-K73</f>
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="N71" s="24">
         <v>1</v>
@@ -17440,16 +17800,36 @@
       <c r="CR72" s="43">
         <v>204</v>
       </c>
-      <c r="CS72" s="43"/>
-      <c r="CT72" s="43"/>
-      <c r="CU72" s="43"/>
-      <c r="CV72" s="43"/>
-      <c r="CW72" s="43"/>
-      <c r="CX72" s="43"/>
-      <c r="CY72" s="43"/>
-      <c r="CZ72" s="43"/>
-      <c r="DA72" s="43"/>
-      <c r="DB72" s="43"/>
+      <c r="CS72" s="43">
+        <v>204</v>
+      </c>
+      <c r="CT72" s="43">
+        <v>204</v>
+      </c>
+      <c r="CU72" s="43">
+        <v>204</v>
+      </c>
+      <c r="CV72" s="43">
+        <v>202</v>
+      </c>
+      <c r="CW72" s="43">
+        <v>202</v>
+      </c>
+      <c r="CX72" s="43">
+        <v>202</v>
+      </c>
+      <c r="CY72" s="43">
+        <v>202</v>
+      </c>
+      <c r="CZ72" s="43">
+        <v>202</v>
+      </c>
+      <c r="DA72" s="43">
+        <v>205</v>
+      </c>
+      <c r="DB72" s="43">
+        <v>200</v>
+      </c>
       <c r="DC72" s="43"/>
       <c r="DD72" s="43"/>
       <c r="DE72" s="43"/>
@@ -17491,15 +17871,15 @@
       </c>
       <c r="K73" s="29">
         <f t="shared" si="43"/>
-        <v>135</v>
+        <v>170</v>
       </c>
       <c r="L73" s="51">
         <f t="shared" si="44"/>
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="M73" s="29">
         <f>K73-K75</f>
-        <v>135</v>
+        <v>170</v>
       </c>
       <c r="N73" s="29">
         <v>1</v>
@@ -18088,16 +18468,36 @@
       <c r="CR74" s="43">
         <v>135</v>
       </c>
-      <c r="CS74" s="43"/>
-      <c r="CT74" s="43"/>
-      <c r="CU74" s="43"/>
-      <c r="CV74" s="43"/>
-      <c r="CW74" s="43"/>
-      <c r="CX74" s="43"/>
-      <c r="CY74" s="43"/>
-      <c r="CZ74" s="43"/>
-      <c r="DA74" s="43"/>
-      <c r="DB74" s="43"/>
+      <c r="CS74" s="43">
+        <v>141</v>
+      </c>
+      <c r="CT74" s="43">
+        <v>147</v>
+      </c>
+      <c r="CU74" s="43">
+        <v>147</v>
+      </c>
+      <c r="CV74" s="43">
+        <v>151</v>
+      </c>
+      <c r="CW74" s="43">
+        <v>155</v>
+      </c>
+      <c r="CX74" s="43">
+        <v>157</v>
+      </c>
+      <c r="CY74" s="43">
+        <v>159</v>
+      </c>
+      <c r="CZ74" s="43">
+        <v>161</v>
+      </c>
+      <c r="DA74" s="43">
+        <v>166</v>
+      </c>
+      <c r="DB74" s="43">
+        <v>170</v>
+      </c>
       <c r="DC74" s="43"/>
       <c r="DD74" s="43"/>
       <c r="DE74" s="43"/>
@@ -18404,15 +18804,15 @@
       </c>
       <c r="K77" s="86">
         <f>MAX(O78:DP78)</f>
-        <v>756</v>
+        <v>778</v>
       </c>
       <c r="L77" s="87">
         <f t="shared" ref="L77:L81" si="50">J77-K77</f>
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="M77" s="86">
         <f>K77-K79</f>
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="N77" s="86">
         <v>9</v>
@@ -18816,7 +19216,7 @@
       <c r="AF78" s="43"/>
       <c r="AG78" s="43"/>
       <c r="AH78" s="43">
-        <f t="shared" ref="AH78:CQ78" si="53">AH18+AH24+AH30+AH36+AH42+AH48+AH54+AH60+AH66+AH72</f>
+        <f t="shared" ref="AH78:CS78" si="53">AH18+AH24+AH30+AH36+AH42+AH48+AH54+AH60+AH66+AH72</f>
         <v>231</v>
       </c>
       <c r="AI78" s="43">
@@ -19064,19 +19464,49 @@
         <v>683</v>
       </c>
       <c r="CR78" s="43">
-        <f>CR18+CR24+CR30+CR36+CR42+CR48+CR54+CR60+CR66+CR72</f>
+        <f t="shared" si="53"/>
         <v>756</v>
       </c>
-      <c r="CS78" s="43"/>
-      <c r="CT78" s="43"/>
-      <c r="CU78" s="43"/>
-      <c r="CV78" s="43"/>
-      <c r="CW78" s="43"/>
-      <c r="CX78" s="43"/>
-      <c r="CY78" s="43"/>
-      <c r="CZ78" s="43"/>
-      <c r="DA78" s="43"/>
-      <c r="DB78" s="43"/>
+      <c r="CS78" s="43">
+        <f t="shared" si="53"/>
+        <v>758</v>
+      </c>
+      <c r="CT78" s="43">
+        <f t="shared" ref="CT78:CZ78" si="54">CT18+CT24+CT30+CT36+CT42+CT48+CT54+CT60+CT66+CT72</f>
+        <v>760</v>
+      </c>
+      <c r="CU78" s="43">
+        <f t="shared" si="54"/>
+        <v>761</v>
+      </c>
+      <c r="CV78" s="43">
+        <f t="shared" si="54"/>
+        <v>761</v>
+      </c>
+      <c r="CW78" s="43">
+        <f t="shared" si="54"/>
+        <v>761</v>
+      </c>
+      <c r="CX78" s="43">
+        <f t="shared" si="54"/>
+        <v>761</v>
+      </c>
+      <c r="CY78" s="43">
+        <f t="shared" si="54"/>
+        <v>763</v>
+      </c>
+      <c r="CZ78" s="43">
+        <f t="shared" si="54"/>
+        <v>770</v>
+      </c>
+      <c r="DA78" s="43">
+        <f>DA18+DA24+DA30+DA36+DA42+DA48+DA54+DA60+DA66+DA72</f>
+        <v>778</v>
+      </c>
+      <c r="DB78" s="43">
+        <f>DB18+DB24+DB30+DB36+DB42+DB48+DB54+DB60+DB66+DB72</f>
+        <v>771</v>
+      </c>
       <c r="DC78" s="43"/>
       <c r="DD78" s="43"/>
       <c r="DE78" s="43"/>
@@ -19112,15 +19542,15 @@
       </c>
       <c r="K79" s="90">
         <f>MAX(O80:DP80)</f>
-        <v>670</v>
+        <v>715</v>
       </c>
       <c r="L79" s="91">
         <f t="shared" si="50"/>
-        <v>238</v>
+        <v>193</v>
       </c>
       <c r="M79" s="90">
         <f>K79-K81</f>
-        <v>670</v>
+        <v>715</v>
       </c>
       <c r="N79" s="88">
         <v>9</v>
@@ -19149,347 +19579,347 @@
         <v>68</v>
       </c>
       <c r="AI79" s="43">
-        <f t="shared" ref="AI79:AN79" si="54">AH79+$N$79</f>
+        <f t="shared" ref="AI79:AN79" si="55">AH79+$N$79</f>
         <v>77</v>
       </c>
       <c r="AJ79" s="43">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>86</v>
       </c>
       <c r="AK79" s="43">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>95</v>
       </c>
       <c r="AL79" s="43">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>104</v>
       </c>
       <c r="AM79" s="43">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>113</v>
       </c>
       <c r="AN79" s="43">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>122</v>
       </c>
       <c r="AO79" s="43">
-        <f t="shared" ref="AO79:BT79" si="55">AN79+$N$79</f>
+        <f t="shared" ref="AO79:BT79" si="56">AN79+$N$79</f>
         <v>131</v>
       </c>
       <c r="AP79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>140</v>
       </c>
       <c r="AQ79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>149</v>
       </c>
       <c r="AR79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>158</v>
       </c>
       <c r="AS79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>167</v>
       </c>
       <c r="AT79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>176</v>
       </c>
       <c r="AU79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>185</v>
       </c>
       <c r="AV79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>194</v>
       </c>
       <c r="AW79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>203</v>
       </c>
       <c r="AX79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>212</v>
       </c>
       <c r="AY79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>221</v>
       </c>
       <c r="AZ79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>230</v>
       </c>
       <c r="BA79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>239</v>
       </c>
       <c r="BB79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>248</v>
       </c>
       <c r="BC79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>257</v>
       </c>
       <c r="BD79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>266</v>
       </c>
       <c r="BE79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>275</v>
       </c>
       <c r="BF79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>284</v>
       </c>
       <c r="BG79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>293</v>
       </c>
       <c r="BH79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>302</v>
       </c>
       <c r="BI79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>311</v>
       </c>
       <c r="BJ79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>320</v>
       </c>
       <c r="BK79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>329</v>
       </c>
       <c r="BL79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>338</v>
       </c>
       <c r="BM79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>347</v>
       </c>
       <c r="BN79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>356</v>
       </c>
       <c r="BO79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>365</v>
       </c>
       <c r="BP79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>374</v>
       </c>
       <c r="BQ79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>383</v>
       </c>
       <c r="BR79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>392</v>
       </c>
       <c r="BS79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>401</v>
       </c>
       <c r="BT79" s="43">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>410</v>
       </c>
       <c r="BU79" s="43">
-        <f t="shared" ref="BU79:CZ79" si="56">BT79+$N$79</f>
+        <f t="shared" ref="BU79:CZ79" si="57">BT79+$N$79</f>
         <v>419</v>
       </c>
       <c r="BV79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>428</v>
       </c>
       <c r="BW79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>437</v>
       </c>
       <c r="BX79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>446</v>
       </c>
       <c r="BY79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>455</v>
       </c>
       <c r="BZ79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>464</v>
       </c>
       <c r="CA79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>473</v>
       </c>
       <c r="CB79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>482</v>
       </c>
       <c r="CC79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>491</v>
       </c>
       <c r="CD79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>500</v>
       </c>
       <c r="CE79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>509</v>
       </c>
       <c r="CF79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>518</v>
       </c>
       <c r="CG79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>527</v>
       </c>
       <c r="CH79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>536</v>
       </c>
       <c r="CI79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>545</v>
       </c>
       <c r="CJ79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>554</v>
       </c>
       <c r="CK79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>563</v>
       </c>
       <c r="CL79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>572</v>
       </c>
       <c r="CM79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>581</v>
       </c>
       <c r="CN79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>590</v>
       </c>
       <c r="CO79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>599</v>
       </c>
       <c r="CP79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>608</v>
       </c>
       <c r="CQ79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>617</v>
       </c>
       <c r="CR79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>626</v>
       </c>
       <c r="CS79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>635</v>
       </c>
       <c r="CT79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>644</v>
       </c>
       <c r="CU79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>653</v>
       </c>
       <c r="CV79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>662</v>
       </c>
       <c r="CW79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>671</v>
       </c>
       <c r="CX79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>680</v>
       </c>
       <c r="CY79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>689</v>
       </c>
       <c r="CZ79" s="43">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>698</v>
       </c>
       <c r="DA79" s="43">
-        <f t="shared" ref="DA79:DH79" si="57">CZ79+$N$79</f>
+        <f t="shared" ref="DA79:DH79" si="58">CZ79+$N$79</f>
         <v>707</v>
       </c>
       <c r="DB79" s="43">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>716</v>
       </c>
       <c r="DC79" s="43">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>725</v>
       </c>
       <c r="DD79" s="43">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>734</v>
       </c>
       <c r="DE79" s="43">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>743</v>
       </c>
       <c r="DF79" s="43">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>752</v>
       </c>
       <c r="DG79" s="43">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>761</v>
       </c>
       <c r="DH79" s="43">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>770</v>
       </c>
       <c r="DI79" s="43">
-        <f t="shared" ref="DI79:DP79" si="58">DH79+$N$79</f>
+        <f t="shared" ref="DI79:DP79" si="59">DH79+$N$79</f>
         <v>779</v>
       </c>
       <c r="DJ79" s="43">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>788</v>
       </c>
       <c r="DK79" s="43">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>797</v>
       </c>
       <c r="DL79" s="43">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>806</v>
       </c>
       <c r="DM79" s="43">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>815</v>
       </c>
       <c r="DN79" s="43">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>824</v>
       </c>
       <c r="DO79" s="43">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>833</v>
       </c>
       <c r="DP79" s="70">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>842</v>
       </c>
     </row>
@@ -19528,267 +19958,297 @@
       <c r="AF80" s="43"/>
       <c r="AG80" s="43"/>
       <c r="AH80" s="43">
-        <f t="shared" ref="AH80:CQ80" si="59">AH20+AH26+AH32+AH38+AH44+AH50+AH56+AH62+AH68+AH74</f>
+        <f t="shared" ref="AH80:CS80" si="60">AH20+AH26+AH32+AH38+AH44+AH50+AH56+AH62+AH68+AH74</f>
         <v>68</v>
       </c>
       <c r="AI80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>70</v>
       </c>
       <c r="AJ80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>71</v>
       </c>
       <c r="AK80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>71</v>
       </c>
       <c r="AL80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>71</v>
       </c>
       <c r="AM80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>71</v>
       </c>
       <c r="AN80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>71</v>
       </c>
       <c r="AO80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>71</v>
       </c>
       <c r="AP80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>71</v>
       </c>
       <c r="AQ80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>72</v>
       </c>
       <c r="AR80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>73</v>
       </c>
       <c r="AS80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>75</v>
       </c>
       <c r="AT80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>75</v>
       </c>
       <c r="AU80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>75</v>
       </c>
       <c r="AV80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>75</v>
       </c>
       <c r="AW80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>76</v>
       </c>
       <c r="AX80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>82</v>
       </c>
       <c r="AY80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>100</v>
       </c>
       <c r="AZ80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>104</v>
       </c>
       <c r="BA80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>106</v>
       </c>
       <c r="BB80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>119</v>
       </c>
       <c r="BC80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>125</v>
       </c>
       <c r="BD80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>160</v>
       </c>
       <c r="BE80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>184</v>
       </c>
       <c r="BF80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>200</v>
       </c>
       <c r="BG80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>226</v>
       </c>
       <c r="BH80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>246</v>
       </c>
       <c r="BI80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>269</v>
       </c>
       <c r="BJ80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>289</v>
       </c>
       <c r="BK80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>313</v>
       </c>
       <c r="BL80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>337</v>
       </c>
       <c r="BM80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>337</v>
       </c>
       <c r="BN80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>337</v>
       </c>
       <c r="BO80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>337</v>
       </c>
       <c r="BP80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>350</v>
       </c>
       <c r="BQ80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>372</v>
       </c>
       <c r="BR80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>393</v>
       </c>
       <c r="BS80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>403</v>
       </c>
       <c r="BT80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>410</v>
       </c>
       <c r="BU80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>420</v>
       </c>
       <c r="BV80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>425</v>
       </c>
       <c r="BW80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>433</v>
       </c>
       <c r="BX80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>448</v>
       </c>
       <c r="BY80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>463</v>
       </c>
       <c r="BZ80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>475</v>
       </c>
       <c r="CA80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>481</v>
       </c>
       <c r="CB80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>493</v>
       </c>
       <c r="CC80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>500</v>
       </c>
       <c r="CD80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>512</v>
       </c>
       <c r="CE80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>519</v>
       </c>
       <c r="CF80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>529</v>
       </c>
       <c r="CG80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>537</v>
       </c>
       <c r="CH80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>549</v>
       </c>
       <c r="CI80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>553</v>
       </c>
       <c r="CJ80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>561</v>
       </c>
       <c r="CK80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>570</v>
       </c>
       <c r="CL80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>578</v>
       </c>
       <c r="CM80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>583</v>
       </c>
       <c r="CN80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>592</v>
       </c>
       <c r="CO80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>598</v>
       </c>
       <c r="CP80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>603</v>
       </c>
       <c r="CQ80" s="43">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>608</v>
       </c>
       <c r="CR80" s="43">
-        <f>CR20+CR26+CR32+CR38+CR44+CR50+CR56+CR62+CR68+CR74</f>
+        <f t="shared" si="60"/>
         <v>670</v>
       </c>
-      <c r="CS80" s="43"/>
-      <c r="CT80" s="43"/>
-      <c r="CU80" s="43"/>
-      <c r="CV80" s="43"/>
-      <c r="CW80" s="43"/>
-      <c r="CX80" s="43"/>
-      <c r="CY80" s="43"/>
-      <c r="CZ80" s="43"/>
-      <c r="DA80" s="43"/>
-      <c r="DB80" s="43"/>
+      <c r="CS80" s="43">
+        <f t="shared" si="60"/>
+        <v>676</v>
+      </c>
+      <c r="CT80" s="43">
+        <f t="shared" ref="CT80:CZ80" si="61">CT20+CT26+CT32+CT38+CT44+CT50+CT56+CT62+CT68+CT74</f>
+        <v>683</v>
+      </c>
+      <c r="CU80" s="43">
+        <f t="shared" si="61"/>
+        <v>683</v>
+      </c>
+      <c r="CV80" s="43">
+        <f t="shared" si="61"/>
+        <v>688</v>
+      </c>
+      <c r="CW80" s="43">
+        <f t="shared" si="61"/>
+        <v>692</v>
+      </c>
+      <c r="CX80" s="43">
+        <f t="shared" si="61"/>
+        <v>694</v>
+      </c>
+      <c r="CY80" s="43">
+        <f t="shared" si="61"/>
+        <v>696</v>
+      </c>
+      <c r="CZ80" s="43">
+        <f t="shared" si="61"/>
+        <v>702</v>
+      </c>
+      <c r="DA80" s="43">
+        <f>DA20+DA26+DA32+DA38+DA44+DA50+DA56+DA62+DA68+DA74</f>
+        <v>709</v>
+      </c>
+      <c r="DB80" s="43">
+        <f>DB20+DB26+DB32+DB38+DB44+DB50+DB56+DB62+DB68+DB74</f>
+        <v>715</v>
+      </c>
       <c r="DC80" s="43"/>
       <c r="DD80" s="43"/>
       <c r="DE80" s="43"/>

</xml_diff>

<commit_message>
Quita reglas parte 1
</commit_message>
<xml_diff>
--- a/UPGRADE 3100-5000.xlsx
+++ b/UPGRADE 3100-5000.xlsx
@@ -1195,8 +1195,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26">
@@ -1237,28 +1237,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1274,8 +1252,69 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1289,31 +1328,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1329,43 +1345,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1378,12 +1380,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -1479,31 +1479,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1515,43 +1533,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1563,67 +1545,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1641,7 +1569,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1873,13 +1873,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1903,7 +1922,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1912,7 +1931,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1932,17 +1951,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1955,31 +1970,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1994,128 +1994,128 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="42" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2738,11 +2738,11 @@
   <dimension ref="A1:DP685"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="I1" workbookViewId="0">
-      <pane xSplit="5745" ySplit="1170" topLeftCell="CL76" activePane="bottomRight"/>
+      <pane xSplit="5745" ySplit="1170" topLeftCell="CS70" activePane="bottomRight"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="DG81" sqref="DG81"/>
+      <selection pane="bottomRight" activeCell="CX75" sqref="CX75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4285714285714" defaultRowHeight="11.25"/>
@@ -5283,15 +5283,15 @@
       </c>
       <c r="K17" s="24">
         <f t="shared" ref="K17:K21" si="0">MAX(AH18:DP18)</f>
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L17" s="49">
         <f t="shared" ref="L17:L21" si="1">J17-K17</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M17" s="24">
         <f>K17-K19</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N17" s="24">
         <v>1</v>
@@ -5615,7 +5615,9 @@
       </c>
       <c r="J18" s="29"/>
       <c r="K18" s="29"/>
-      <c r="L18" s="51"/>
+      <c r="L18" s="51">
+        <v>0</v>
+      </c>
       <c r="M18" s="29"/>
       <c r="N18" s="29"/>
       <c r="O18" s="52"/>
@@ -5864,9 +5866,15 @@
       <c r="DH18" s="60">
         <v>89</v>
       </c>
-      <c r="DI18" s="60"/>
-      <c r="DJ18" s="60"/>
-      <c r="DK18" s="60"/>
+      <c r="DI18" s="60">
+        <v>89</v>
+      </c>
+      <c r="DJ18" s="60">
+        <v>91</v>
+      </c>
+      <c r="DK18" s="60">
+        <v>91</v>
+      </c>
       <c r="DL18" s="60"/>
       <c r="DM18" s="60"/>
       <c r="DN18" s="60"/>
@@ -5907,15 +5915,15 @@
       </c>
       <c r="K19" s="29">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L19" s="51">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M19" s="29">
         <f>K19-K21</f>
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N19" s="29">
         <v>1</v>
@@ -6486,9 +6494,15 @@
       <c r="DH20" s="43">
         <v>85</v>
       </c>
-      <c r="DI20" s="43"/>
-      <c r="DJ20" s="43"/>
-      <c r="DK20" s="43"/>
+      <c r="DI20" s="43">
+        <v>85</v>
+      </c>
+      <c r="DJ20" s="43">
+        <v>86</v>
+      </c>
+      <c r="DK20" s="43">
+        <v>86</v>
+      </c>
       <c r="DL20" s="43"/>
       <c r="DM20" s="43"/>
       <c r="DN20" s="43"/>
@@ -6783,19 +6797,19 @@
         <v>54</v>
       </c>
       <c r="J23" s="24">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="K23" s="24">
         <f t="shared" ref="K23:K27" si="7">MAX(AH24:DP24)</f>
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="L23" s="49">
         <f t="shared" ref="L23:L27" si="8">J23-K23</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="M23" s="24">
         <f>K23-K25</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="N23" s="24">
         <v>1</v>
@@ -7041,7 +7055,9 @@
       </c>
       <c r="J24" s="29"/>
       <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
+      <c r="L24" s="29">
+        <v>7</v>
+      </c>
       <c r="M24" s="29"/>
       <c r="N24" s="29"/>
       <c r="O24" s="43"/>
@@ -7290,9 +7306,15 @@
       <c r="DH24" s="43">
         <v>69</v>
       </c>
-      <c r="DI24" s="43"/>
-      <c r="DJ24" s="43"/>
-      <c r="DK24" s="43"/>
+      <c r="DI24" s="43">
+        <v>69</v>
+      </c>
+      <c r="DJ24" s="43">
+        <v>70</v>
+      </c>
+      <c r="DK24" s="43">
+        <v>76</v>
+      </c>
       <c r="DL24" s="43"/>
       <c r="DM24" s="43"/>
       <c r="DN24" s="43"/>
@@ -7325,7 +7347,7 @@
       </c>
       <c r="J25" s="29">
         <f>J23</f>
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="K25" s="29">
         <f t="shared" si="7"/>
@@ -7333,7 +7355,7 @@
       </c>
       <c r="L25" s="51">
         <f t="shared" si="8"/>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="M25" s="29">
         <f>K25-K27</f>
@@ -7830,9 +7852,15 @@
       <c r="DH26" s="43">
         <v>64</v>
       </c>
-      <c r="DI26" s="43"/>
-      <c r="DJ26" s="43"/>
-      <c r="DK26" s="43"/>
+      <c r="DI26" s="43">
+        <v>64</v>
+      </c>
+      <c r="DJ26" s="43">
+        <v>64</v>
+      </c>
+      <c r="DK26" s="43">
+        <v>64</v>
+      </c>
       <c r="DL26" s="43"/>
       <c r="DM26" s="43"/>
       <c r="DN26" s="43"/>
@@ -7857,7 +7885,7 @@
       </c>
       <c r="J27" s="29">
         <f>J25</f>
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="K27" s="29">
         <f t="shared" si="7"/>
@@ -7865,7 +7893,7 @@
       </c>
       <c r="L27" s="51">
         <f t="shared" si="8"/>
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="M27" s="29"/>
       <c r="N27" s="29"/>
@@ -8127,19 +8155,19 @@
         <v>54</v>
       </c>
       <c r="J29" s="24">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="K29" s="24">
         <f t="shared" ref="K29:K33" si="11">MAX(AH30:DP30)</f>
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="L29" s="49">
         <f t="shared" ref="L29:L33" si="12">J29-K29</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="M29" s="24">
         <f>K29-K31</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="N29" s="24">
         <v>2</v>
@@ -8505,7 +8533,9 @@
       </c>
       <c r="J30" s="29"/>
       <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
+      <c r="L30" s="29">
+        <v>10</v>
+      </c>
       <c r="M30" s="29"/>
       <c r="N30" s="29"/>
       <c r="O30" s="43"/>
@@ -8754,9 +8784,15 @@
       <c r="DH30" s="43">
         <v>141</v>
       </c>
-      <c r="DI30" s="43"/>
-      <c r="DJ30" s="43"/>
-      <c r="DK30" s="43"/>
+      <c r="DI30" s="43">
+        <v>141</v>
+      </c>
+      <c r="DJ30" s="43">
+        <v>141</v>
+      </c>
+      <c r="DK30" s="43">
+        <v>152</v>
+      </c>
       <c r="DL30" s="43"/>
       <c r="DM30" s="43"/>
       <c r="DN30" s="43"/>
@@ -8789,19 +8825,19 @@
       </c>
       <c r="J31" s="29">
         <f>J29</f>
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="K31" s="29">
         <f t="shared" si="11"/>
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L31" s="51">
         <f t="shared" si="12"/>
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M31" s="29">
         <f>K31-K33</f>
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="N31" s="29">
         <v>2</v>
@@ -9414,9 +9450,15 @@
       <c r="DH32" s="43">
         <v>137</v>
       </c>
-      <c r="DI32" s="43"/>
-      <c r="DJ32" s="43"/>
-      <c r="DK32" s="43"/>
+      <c r="DI32" s="43">
+        <v>137</v>
+      </c>
+      <c r="DJ32" s="43">
+        <v>137</v>
+      </c>
+      <c r="DK32" s="43">
+        <v>138</v>
+      </c>
       <c r="DL32" s="43"/>
       <c r="DM32" s="43"/>
       <c r="DN32" s="43"/>
@@ -9439,7 +9481,7 @@
       <c r="I33" s="52"/>
       <c r="J33" s="29">
         <f>J31</f>
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="K33" s="29">
         <f t="shared" si="11"/>
@@ -9447,7 +9489,7 @@
       </c>
       <c r="L33" s="51">
         <f t="shared" si="12"/>
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="M33" s="29"/>
       <c r="N33" s="29"/>
@@ -9707,19 +9749,19 @@
         <v>54</v>
       </c>
       <c r="J35" s="24">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="K35" s="24">
         <f t="shared" ref="K35:K39" si="18">MAX(AH36:DP36)</f>
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="L35" s="49">
         <f t="shared" ref="L35:L39" si="19">J35-K35</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M35" s="24">
         <f>K35-K37</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="N35" s="24">
         <v>1</v>
@@ -10016,7 +10058,9 @@
       </c>
       <c r="J36" s="29"/>
       <c r="K36" s="29"/>
-      <c r="L36" s="29"/>
+      <c r="L36" s="29">
+        <v>11</v>
+      </c>
       <c r="M36" s="29"/>
       <c r="N36" s="29"/>
       <c r="O36" s="43"/>
@@ -10265,9 +10309,15 @@
       <c r="DH36" s="43">
         <v>46</v>
       </c>
-      <c r="DI36" s="43"/>
-      <c r="DJ36" s="43"/>
-      <c r="DK36" s="43"/>
+      <c r="DI36" s="43">
+        <v>46</v>
+      </c>
+      <c r="DJ36" s="43">
+        <v>47</v>
+      </c>
+      <c r="DK36" s="43">
+        <v>51</v>
+      </c>
       <c r="DL36" s="43"/>
       <c r="DM36" s="43"/>
       <c r="DN36" s="43"/>
@@ -10298,7 +10348,7 @@
       </c>
       <c r="J37" s="29">
         <f>J35</f>
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="K37" s="29">
         <f t="shared" si="18"/>
@@ -10306,7 +10356,7 @@
       </c>
       <c r="L37" s="51">
         <f t="shared" si="19"/>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="M37" s="29">
         <f>K37-K39</f>
@@ -10854,9 +10904,15 @@
       <c r="DH38" s="43">
         <v>44</v>
       </c>
-      <c r="DI38" s="43"/>
-      <c r="DJ38" s="43"/>
-      <c r="DK38" s="43"/>
+      <c r="DI38" s="43">
+        <v>44</v>
+      </c>
+      <c r="DJ38" s="43">
+        <v>44</v>
+      </c>
+      <c r="DK38" s="43">
+        <v>44</v>
+      </c>
       <c r="DL38" s="43"/>
       <c r="DM38" s="43"/>
       <c r="DN38" s="43"/>
@@ -10881,7 +10937,7 @@
       </c>
       <c r="J39" s="29">
         <f>J37</f>
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="K39" s="29">
         <f t="shared" si="18"/>
@@ -10889,7 +10945,7 @@
       </c>
       <c r="L39" s="51">
         <f t="shared" si="19"/>
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="M39" s="29"/>
       <c r="N39" s="29"/>
@@ -11149,19 +11205,19 @@
         <v>54</v>
       </c>
       <c r="J41" s="24">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K41" s="24">
         <f t="shared" ref="K41:K45" si="23">MAX(AH42:DP42)</f>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L41" s="49">
         <f t="shared" ref="L41:L45" si="24">J41-K41</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M41" s="24">
         <f>K41-K43</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N41" s="24">
         <v>1</v>
@@ -11458,7 +11514,9 @@
       </c>
       <c r="J42" s="29"/>
       <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
+      <c r="L42" s="29">
+        <v>6</v>
+      </c>
       <c r="M42" s="29"/>
       <c r="N42" s="29"/>
       <c r="O42" s="43"/>
@@ -11703,9 +11761,15 @@
       <c r="DH42" s="43">
         <v>52</v>
       </c>
-      <c r="DI42" s="43"/>
-      <c r="DJ42" s="43"/>
-      <c r="DK42" s="43"/>
+      <c r="DI42" s="43">
+        <v>52</v>
+      </c>
+      <c r="DJ42" s="43">
+        <v>52</v>
+      </c>
+      <c r="DK42" s="43">
+        <v>54</v>
+      </c>
       <c r="DL42" s="43"/>
       <c r="DM42" s="43"/>
       <c r="DN42" s="43"/>
@@ -11736,7 +11800,7 @@
       </c>
       <c r="J43" s="29">
         <f>J41</f>
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K43" s="29">
         <f t="shared" si="23"/>
@@ -11744,7 +11808,7 @@
       </c>
       <c r="L43" s="51">
         <f t="shared" si="24"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M43" s="29">
         <f>K43-K45</f>
@@ -12288,9 +12352,15 @@
       <c r="DH44" s="43">
         <v>49</v>
       </c>
-      <c r="DI44" s="43"/>
-      <c r="DJ44" s="43"/>
-      <c r="DK44" s="43"/>
+      <c r="DI44" s="43">
+        <v>49</v>
+      </c>
+      <c r="DJ44" s="43">
+        <v>49</v>
+      </c>
+      <c r="DK44" s="43">
+        <v>49</v>
+      </c>
       <c r="DL44" s="43"/>
       <c r="DM44" s="43"/>
       <c r="DN44" s="43"/>
@@ -12315,7 +12385,7 @@
       </c>
       <c r="J45" s="29">
         <f>J43</f>
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K45" s="29">
         <f t="shared" si="23"/>
@@ -12323,7 +12393,7 @@
       </c>
       <c r="L45" s="51">
         <f t="shared" si="24"/>
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M45" s="29"/>
       <c r="N45" s="29"/>
@@ -12583,7 +12653,7 @@
         <v>54</v>
       </c>
       <c r="J47" s="24">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="K47" s="24">
         <f t="shared" ref="K47:K51" si="28">MAX(AH48:DP48)</f>
@@ -12591,7 +12661,7 @@
       </c>
       <c r="L47" s="49">
         <f t="shared" ref="L47:L51" si="29">J47-K47</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="M47" s="24">
         <f>K47-K49</f>
@@ -12958,7 +13028,9 @@
       </c>
       <c r="J48" s="29"/>
       <c r="K48" s="29"/>
-      <c r="L48" s="29"/>
+      <c r="L48" s="29">
+        <v>3</v>
+      </c>
       <c r="M48" s="29"/>
       <c r="N48" s="29"/>
       <c r="O48" s="43"/>
@@ -13203,9 +13275,15 @@
       <c r="DH48" s="43">
         <v>142</v>
       </c>
-      <c r="DI48" s="43"/>
-      <c r="DJ48" s="43"/>
-      <c r="DK48" s="43"/>
+      <c r="DI48" s="43">
+        <v>142</v>
+      </c>
+      <c r="DJ48" s="43">
+        <v>143</v>
+      </c>
+      <c r="DK48" s="43">
+        <v>145</v>
+      </c>
       <c r="DL48" s="43"/>
       <c r="DM48" s="43"/>
       <c r="DN48" s="43"/>
@@ -13236,7 +13314,7 @@
       </c>
       <c r="J49" s="29">
         <f>J47</f>
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="K49" s="29">
         <f t="shared" si="28"/>
@@ -13244,7 +13322,7 @@
       </c>
       <c r="L49" s="51">
         <f t="shared" si="29"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="M49" s="29">
         <f>K49-K51</f>
@@ -13854,9 +13932,15 @@
       <c r="DH50" s="43">
         <v>134</v>
       </c>
-      <c r="DI50" s="43"/>
-      <c r="DJ50" s="43"/>
-      <c r="DK50" s="43"/>
+      <c r="DI50" s="43">
+        <v>134</v>
+      </c>
+      <c r="DJ50" s="43">
+        <v>134</v>
+      </c>
+      <c r="DK50" s="43">
+        <v>134</v>
+      </c>
       <c r="DL50" s="43"/>
       <c r="DM50" s="43"/>
       <c r="DN50" s="43"/>
@@ -13881,7 +13965,7 @@
       </c>
       <c r="J51" s="29">
         <f>J49</f>
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="K51" s="29">
         <f t="shared" si="28"/>
@@ -13889,7 +13973,7 @@
       </c>
       <c r="L51" s="51">
         <f t="shared" si="29"/>
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="M51" s="29"/>
       <c r="N51" s="29"/>
@@ -14149,19 +14233,19 @@
         <v>54</v>
       </c>
       <c r="J53" s="24">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K53" s="24">
         <f t="shared" ref="K53:K57" si="35">MAX(AH54:DP54)</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="L53" s="49">
         <f t="shared" ref="L53:L57" si="36">J53-K53</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M53" s="24">
         <f>K53-K55</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N53" s="24">
         <v>1</v>
@@ -14383,7 +14467,9 @@
       </c>
       <c r="J54" s="29"/>
       <c r="K54" s="29"/>
-      <c r="L54" s="29"/>
+      <c r="L54" s="29">
+        <v>3</v>
+      </c>
       <c r="M54" s="29"/>
       <c r="N54" s="29"/>
       <c r="O54" s="43"/>
@@ -14548,9 +14634,15 @@
       <c r="DH54" s="43">
         <v>24</v>
       </c>
-      <c r="DI54" s="43"/>
-      <c r="DJ54" s="43"/>
-      <c r="DK54" s="43"/>
+      <c r="DI54" s="43">
+        <v>24</v>
+      </c>
+      <c r="DJ54" s="43">
+        <v>24</v>
+      </c>
+      <c r="DK54" s="43">
+        <v>28</v>
+      </c>
       <c r="DL54" s="43"/>
       <c r="DM54" s="43"/>
       <c r="DN54" s="43"/>
@@ -14581,19 +14673,19 @@
       </c>
       <c r="J55" s="29">
         <f>J53</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K55" s="29">
         <f t="shared" si="35"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L55" s="51">
         <f t="shared" si="36"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M55" s="29">
         <f>K55-K57</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N55" s="29">
         <v>1</v>
@@ -14978,9 +15070,15 @@
       <c r="DH56" s="43">
         <v>24</v>
       </c>
-      <c r="DI56" s="43"/>
-      <c r="DJ56" s="43"/>
-      <c r="DK56" s="43"/>
+      <c r="DI56" s="43">
+        <v>24</v>
+      </c>
+      <c r="DJ56" s="43">
+        <v>24</v>
+      </c>
+      <c r="DK56" s="43">
+        <v>25</v>
+      </c>
       <c r="DL56" s="43"/>
       <c r="DM56" s="43"/>
       <c r="DN56" s="43"/>
@@ -15005,7 +15103,7 @@
       </c>
       <c r="J57" s="29">
         <f>J55</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K57" s="29">
         <f t="shared" si="35"/>
@@ -15013,7 +15111,7 @@
       </c>
       <c r="L57" s="51">
         <f t="shared" si="36"/>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M57" s="29"/>
       <c r="N57" s="29"/>
@@ -15277,11 +15375,11 @@
       </c>
       <c r="K59" s="24">
         <f t="shared" ref="K59:K63" si="39">MAX(AH60:DP60)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L59" s="49">
         <f t="shared" ref="L59:L63" si="40">J59-K59</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M59" s="24">
         <f>K59-K61</f>
@@ -15433,7 +15531,9 @@
       </c>
       <c r="J60" s="29"/>
       <c r="K60" s="29"/>
-      <c r="L60" s="29"/>
+      <c r="L60" s="29">
+        <v>0</v>
+      </c>
       <c r="M60" s="29"/>
       <c r="N60" s="29"/>
       <c r="O60" s="43"/>
@@ -15598,9 +15698,15 @@
       <c r="DH60" s="43">
         <v>8</v>
       </c>
-      <c r="DI60" s="43"/>
-      <c r="DJ60" s="43"/>
-      <c r="DK60" s="43"/>
+      <c r="DI60" s="43">
+        <v>8</v>
+      </c>
+      <c r="DJ60" s="43">
+        <v>8</v>
+      </c>
+      <c r="DK60" s="43">
+        <v>10</v>
+      </c>
       <c r="DL60" s="43"/>
       <c r="DM60" s="43"/>
       <c r="DN60" s="43"/>
@@ -15635,15 +15741,15 @@
       </c>
       <c r="K61" s="29">
         <f t="shared" si="39"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L61" s="51">
         <f t="shared" si="40"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M61" s="29">
         <f>K61-K63</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N61" s="29">
         <v>0</v>
@@ -16006,9 +16112,15 @@
       <c r="DH62" s="43">
         <v>8</v>
       </c>
-      <c r="DI62" s="43"/>
-      <c r="DJ62" s="43"/>
-      <c r="DK62" s="43"/>
+      <c r="DI62" s="43">
+        <v>8</v>
+      </c>
+      <c r="DJ62" s="43">
+        <v>8</v>
+      </c>
+      <c r="DK62" s="43">
+        <v>9</v>
+      </c>
       <c r="DL62" s="43"/>
       <c r="DM62" s="43"/>
       <c r="DN62" s="43"/>
@@ -16447,7 +16559,9 @@
       </c>
       <c r="J66" s="29"/>
       <c r="K66" s="29"/>
-      <c r="L66" s="29"/>
+      <c r="L66" s="29">
+        <v>0</v>
+      </c>
       <c r="M66" s="29"/>
       <c r="N66" s="29"/>
       <c r="O66" s="43"/>
@@ -16604,9 +16718,15 @@
       <c r="DH66" s="43">
         <v>2</v>
       </c>
-      <c r="DI66" s="43"/>
-      <c r="DJ66" s="43"/>
-      <c r="DK66" s="43"/>
+      <c r="DI66" s="43">
+        <v>2</v>
+      </c>
+      <c r="DJ66" s="43">
+        <v>2</v>
+      </c>
+      <c r="DK66" s="43">
+        <v>2</v>
+      </c>
       <c r="DL66" s="43"/>
       <c r="DM66" s="43"/>
       <c r="DN66" s="43"/>
@@ -16938,9 +17058,15 @@
       <c r="DH68" s="43">
         <v>2</v>
       </c>
-      <c r="DI68" s="43"/>
-      <c r="DJ68" s="43"/>
-      <c r="DK68" s="43"/>
+      <c r="DI68" s="43">
+        <v>2</v>
+      </c>
+      <c r="DJ68" s="43">
+        <v>2</v>
+      </c>
+      <c r="DK68" s="43">
+        <v>2</v>
+      </c>
       <c r="DL68" s="43"/>
       <c r="DM68" s="43"/>
       <c r="DN68" s="43"/>
@@ -17233,7 +17359,7 @@
         <v>54</v>
       </c>
       <c r="J71" s="24">
-        <v>274</v>
+        <v>134</v>
       </c>
       <c r="K71" s="24">
         <f t="shared" ref="K71:K75" si="43">MAX(AH72:DP72)</f>
@@ -17241,11 +17367,11 @@
       </c>
       <c r="L71" s="49">
         <f t="shared" ref="L71:L75" si="44">J71-K71</f>
-        <v>69</v>
+        <v>-71</v>
       </c>
       <c r="M71" s="24">
         <f>K71-K73</f>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="N71" s="24">
         <v>1</v>
@@ -17629,7 +17755,9 @@
       </c>
       <c r="J72" s="29"/>
       <c r="K72" s="29"/>
-      <c r="L72" s="29"/>
+      <c r="L72" s="29">
+        <v>5</v>
+      </c>
       <c r="M72" s="29"/>
       <c r="N72" s="29"/>
       <c r="O72" s="43"/>
@@ -17874,9 +18002,15 @@
       <c r="DH72" s="43">
         <v>205</v>
       </c>
-      <c r="DI72" s="43"/>
-      <c r="DJ72" s="43"/>
-      <c r="DK72" s="43"/>
+      <c r="DI72" s="43">
+        <v>205</v>
+      </c>
+      <c r="DJ72" s="43">
+        <v>205</v>
+      </c>
+      <c r="DK72" s="43">
+        <v>129</v>
+      </c>
       <c r="DL72" s="43"/>
       <c r="DM72" s="43"/>
       <c r="DN72" s="43"/>
@@ -17905,19 +18039,19 @@
       </c>
       <c r="J73" s="29">
         <f>J71</f>
-        <v>274</v>
+        <v>134</v>
       </c>
       <c r="K73" s="29">
         <f t="shared" si="43"/>
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="L73" s="51">
         <f t="shared" si="44"/>
-        <v>80</v>
+        <v>-67</v>
       </c>
       <c r="M73" s="29">
         <f>K73-K75</f>
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="N73" s="29">
         <v>1</v>
@@ -18544,9 +18678,15 @@
       <c r="DH74" s="43">
         <v>194</v>
       </c>
-      <c r="DI74" s="43"/>
-      <c r="DJ74" s="43"/>
-      <c r="DK74" s="43"/>
+      <c r="DI74" s="43">
+        <v>197</v>
+      </c>
+      <c r="DJ74" s="43">
+        <v>201</v>
+      </c>
+      <c r="DK74" s="43">
+        <v>119</v>
+      </c>
       <c r="DL74" s="43"/>
       <c r="DM74" s="43"/>
       <c r="DN74" s="43"/>
@@ -18571,7 +18711,7 @@
       </c>
       <c r="J75" s="29">
         <f>J73</f>
-        <v>274</v>
+        <v>134</v>
       </c>
       <c r="K75" s="29">
         <f t="shared" si="43"/>
@@ -18579,7 +18719,7 @@
       </c>
       <c r="L75" s="51">
         <f t="shared" si="44"/>
-        <v>274</v>
+        <v>134</v>
       </c>
       <c r="M75" s="29"/>
       <c r="N75" s="29"/>
@@ -18840,19 +18980,19 @@
       </c>
       <c r="J77" s="75">
         <f>J17+J23+J29+J35+J41+J47+J53+J59+J65+J71</f>
-        <v>908</v>
+        <v>802</v>
       </c>
       <c r="K77" s="86">
         <f>MAX(O78:DP78)</f>
-        <v>778</v>
+        <v>783</v>
       </c>
       <c r="L77" s="87">
         <f t="shared" ref="L77:L81" si="50">J77-K77</f>
-        <v>130</v>
+        <v>19</v>
       </c>
       <c r="M77" s="86">
         <f>K77-K79</f>
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N77" s="86">
         <v>9</v>
@@ -19571,9 +19711,18 @@
         <f t="shared" si="55"/>
         <v>778</v>
       </c>
-      <c r="DI78" s="43"/>
-      <c r="DJ78" s="43"/>
-      <c r="DK78" s="43"/>
+      <c r="DI78" s="43">
+        <f>DI18+DI24+DI30+DI36+DI42+DI48+DI54+DI60+DI66+DI72</f>
+        <v>778</v>
+      </c>
+      <c r="DJ78" s="43">
+        <f>DJ18+DJ24+DJ30+DJ36+DJ42+DJ48+DJ54+DJ60+DJ66+DJ72</f>
+        <v>783</v>
+      </c>
+      <c r="DK78" s="43">
+        <f>DK18+DK24+DK30+DK36+DK42+DK48+DK54+DK60+DK66+DK72</f>
+        <v>738</v>
+      </c>
       <c r="DL78" s="43"/>
       <c r="DM78" s="43"/>
       <c r="DN78" s="43"/>
@@ -19596,19 +19745,19 @@
       </c>
       <c r="J79" s="90">
         <f>J77</f>
-        <v>908</v>
+        <v>802</v>
       </c>
       <c r="K79" s="90">
         <f>MAX(O80:DP80)</f>
-        <v>741</v>
+        <v>749</v>
       </c>
       <c r="L79" s="91">
         <f t="shared" si="50"/>
-        <v>167</v>
+        <v>53</v>
       </c>
       <c r="M79" s="90">
         <f>K79-K81</f>
-        <v>741</v>
+        <v>749</v>
       </c>
       <c r="N79" s="88">
         <v>9</v>
@@ -20331,9 +20480,18 @@
         <f t="shared" si="63"/>
         <v>741</v>
       </c>
-      <c r="DI80" s="43"/>
-      <c r="DJ80" s="43"/>
-      <c r="DK80" s="43"/>
+      <c r="DI80" s="43">
+        <f>DI20+DI26+DI32+DI38+DI44+DI50+DI56+DI62+DI68+DI74</f>
+        <v>744</v>
+      </c>
+      <c r="DJ80" s="43">
+        <f>DJ20+DJ26+DJ32+DJ38+DJ44+DJ50+DJ56+DJ62+DJ68+DJ74</f>
+        <v>749</v>
+      </c>
+      <c r="DK80" s="43">
+        <f>DK20+DK26+DK32+DK38+DK44+DK50+DK56+DK62+DK68+DK74</f>
+        <v>670</v>
+      </c>
       <c r="DL80" s="43"/>
       <c r="DM80" s="43"/>
       <c r="DN80" s="43"/>
@@ -20354,7 +20512,7 @@
       </c>
       <c r="J81" s="90">
         <f>J79</f>
-        <v>908</v>
+        <v>802</v>
       </c>
       <c r="K81" s="90">
         <f>MAX(AH82:DP82)</f>
@@ -20362,7 +20520,7 @@
       </c>
       <c r="L81" s="91">
         <f t="shared" si="50"/>
-        <v>908</v>
+        <v>802</v>
       </c>
       <c r="M81" s="90"/>
       <c r="N81" s="88"/>

</xml_diff>